<commit_message>
Adding documentation, backlog and sprint info
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="53">
   <si>
     <t>Id</t>
   </si>
@@ -165,6 +165,24 @@
   </si>
   <si>
     <t>Effort</t>
+  </si>
+  <si>
+    <t>Implement speed slider</t>
+  </si>
+  <si>
+    <t>Implement slider to control bpm of the song</t>
+  </si>
+  <si>
+    <t>Problems with wav file format</t>
+  </si>
+  <si>
+    <t>Should implement normalizer of wav files</t>
+  </si>
+  <si>
+    <t>Too much clicking on track to add wav file cause System.ArgumentOutOfRangeException</t>
+  </si>
+  <si>
+    <t>Probably because dobule clicked on same position</t>
   </si>
 </sst>
 </file>
@@ -618,17 +636,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
+    <col min="2" max="2" width="57.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -667,7 +686,9 @@
       <c r="E2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -686,7 +707,9 @@
       <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -705,7 +728,9 @@
       <c r="E4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -724,7 +749,9 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3">
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -743,7 +770,9 @@
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -762,7 +791,9 @@
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -781,7 +812,9 @@
       <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -800,7 +833,9 @@
       <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -819,7 +854,9 @@
       <c r="E10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -838,7 +875,9 @@
       <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -857,7 +896,9 @@
       <c r="E12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -876,7 +917,9 @@
       <c r="E13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
@@ -895,7 +938,9 @@
       <c r="E14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
@@ -914,7 +959,9 @@
       <c r="E15" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -933,7 +980,9 @@
       <c r="E16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -952,7 +1001,9 @@
       <c r="E17" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3">
+        <v>3</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
@@ -971,40 +1022,72 @@
       <c r="E18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3"/>
+      <c r="B19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="3">
+        <v>13</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
+      <c r="B21" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">

</xml_diff>

<commit_message>
Daily standup, sprint 5 day 8
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -234,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -284,22 +284,49 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -313,13 +340,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="8" tint="-0.499984740745262"/>
@@ -655,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,22 +726,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="12" t="s">
         <v>46</v>
       </c>
     </row>
@@ -755,7 +809,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A25" si="0">A4+1</f>
+        <f t="shared" ref="A5:A24" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -1173,27 +1227,57 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="4" t="s">
+        <f>A23+1</f>
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="D25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="3">
         <v>20</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D1048576">
+  <conditionalFormatting sqref="D1:D24 D26:D1048576">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"In progress"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+      <formula>"Not sprint ready"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+      <formula>"Sprint ready"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -1211,7 +1295,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>"Sprint ready, Not sprint ready,Completed,In progress,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C27">
       <formula1>"High,Medium,Low,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated sprint info and backlog
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D7" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,164 +791,164 @@
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>30</v>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f t="shared" ref="A5:A24" si="0">A4+1</f>
+        <f>A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f t="shared" si="0"/>
+        <f>A5+1</f>
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F6" s="3">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f t="shared" si="0"/>
+        <f>A6+1</f>
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>31</v>
+      <c r="B7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f t="shared" si="0"/>
+        <f>A7+1</f>
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="F8" s="3">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f t="shared" si="0"/>
+        <f>A8+1</f>
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3">
         <v>20</v>
-      </c>
-      <c r="F9" s="3">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f t="shared" si="0"/>
+        <f>A9+1</f>
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="F10" s="3">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f t="shared" si="0"/>
+        <f>A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="F11" s="3">
         <v>8</v>
@@ -956,167 +956,165 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f t="shared" si="0"/>
+        <f>A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>26</v>
+      <c r="E12" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="F12" s="3">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f t="shared" si="0"/>
+        <f>A12+1</f>
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>45</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E13" s="6"/>
       <c r="F13" s="3">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f t="shared" si="0"/>
+        <f>A13+1</f>
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>33</v>
+        <v>8</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="F14" s="3">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f t="shared" si="0"/>
+        <f>A14+1</f>
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F15" s="3">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
+        <f>A15+1</f>
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="F16" s="3">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f t="shared" si="0"/>
+        <f>A16+1</f>
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F17" s="3">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f t="shared" si="0"/>
+        <f>A17+1</f>
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F18" s="3">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f t="shared" si="0"/>
+        <f>A18+1</f>
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>48</v>
+        <v>17</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="F19" s="3">
         <v>13</v>
@@ -1124,41 +1122,41 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f t="shared" si="0"/>
+        <f>A19+1</f>
         <v>19</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="8" t="s">
+      <c r="B20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="6" t="s">
-        <v>50</v>
+      <c r="E20" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="F20" s="3">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f t="shared" si="0"/>
+        <f>A20+1</f>
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>52</v>
+        <v>16</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="F21" s="3">
         <v>8</v>
@@ -1166,63 +1164,65 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f t="shared" si="0"/>
+        <f>A21+1</f>
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>54</v>
+        <v>16</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="F22" s="3">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f t="shared" si="0"/>
+        <f>A22+1</f>
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>29</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="6"/>
+        <v>16</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="F23" s="3">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f t="shared" si="0"/>
+        <f>A23+1</f>
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="F24" s="3">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1263,6 +1263,9 @@
       <c r="F27" s="2"/>
     </row>
   </sheetData>
+  <sortState ref="A2:F27">
+    <sortCondition ref="D2:D27"/>
+  </sortState>
   <conditionalFormatting sqref="D1:D24 D26:D1048576">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"In progress"</formula>

</xml_diff>

<commit_message>
Added new story to backlog and assinging task
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
   <si>
     <t>Id</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Changing of frequency, etc...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implement frequention changing per track </t>
+  </si>
+  <si>
+    <t>Changing tone of the track in add dialog - referencing 24</t>
   </si>
 </sst>
 </file>
@@ -711,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +773,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <f>A2+1</f>
+        <f t="shared" ref="A3:A26" si="0">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -788,7 +794,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <f>A3+1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -809,7 +815,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <f>A4+1</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -830,7 +836,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <f>A5+1</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
@@ -851,7 +857,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <f>A6+1</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
@@ -872,7 +878,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f>A7+1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -893,7 +899,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <f>A8+1</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -914,7 +920,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <f>A9+1</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -933,9 +939,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <f>A10+1</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -956,7 +962,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f>A11+1</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -977,7 +983,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <f>A12+1</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -996,7 +1002,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <f>A13+1</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1017,7 +1023,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <f>A14+1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="8" t="s">
@@ -1038,7 +1044,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f>A15+1</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1059,7 +1065,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <f>A16+1</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="8" t="s">
@@ -1080,7 +1086,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <f>A17+1</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -1101,7 +1107,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <f>A18+1</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1122,7 +1128,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f>A19+1</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -1141,9 +1147,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <f>A20+1</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="8" t="s">
@@ -1164,7 +1170,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <f>A21+1</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -1185,7 +1191,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <f>A22+1</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -1206,7 +1212,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <f>A23+1</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -1227,8 +1233,8 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <f>A23+1</f>
-        <v>23</v>
+        <f t="shared" si="0"/>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>58</v>
@@ -1247,12 +1253,25 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
+      <c r="A26" s="9">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>

</xml_diff>

<commit_message>
Added few thing in sprint info and restyling backlog
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -354,7 +354,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.14996795556505021"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="8" tint="-0.499984740745262"/>
@@ -407,6 +467,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF8A0000"/>
+      <color rgb="FF990000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -717,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E24" sqref="E23:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1240,7 +1306,7 @@
         <v>58</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>16</v>
@@ -1286,31 +1352,42 @@
     <sortCondition ref="D2:D27"/>
   </sortState>
   <conditionalFormatting sqref="D1:D24 D26:D1048576">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Sprint ready"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Low">
+      <formula>NOT(ISERROR(SEARCH("Low",C1)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"High"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Created new sprint info file and backlog refinement
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="66">
   <si>
     <t>Id</t>
   </si>
@@ -788,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,19 +827,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F2" s="8">
         <v>8</v>
@@ -847,20 +847,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
-        <f>A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>7</v>
+      <c r="D3" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F3" s="8">
         <v>8</v>
@@ -868,20 +867,19 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
-        <f>A3+1</f>
-        <v>3</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="F4" s="8">
         <v>13</v>
@@ -889,333 +887,315 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
-        <f>A4+1</f>
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>31</v>
+        <v>22</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="F5" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
-        <f>A5+1</f>
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="F6" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
-        <f>A6+1</f>
-        <v>6</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>7</v>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="8">
         <v>20</v>
       </c>
-      <c r="F7" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <f>A7+1</f>
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>44</v>
+        <v>16</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="F8" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <f>A8+1</f>
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" s="8">
         <v>8</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <f>A9+1</f>
-        <v>9</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <f>A10+1</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>50</v>
+        <v>17</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F11" s="8">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <f>A11+1</f>
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>51</v>
+        <v>17</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="F12" s="8">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <f>A12+1</f>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <f>A13+1</f>
+        <v>18</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="8">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="10" t="s">
+    </row>
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>10</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>31</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <f>A14+1</f>
-        <v>14</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>29</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <f>A15+1</f>
-        <v>15</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>18</v>
+      <c r="E16" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="F16" s="8">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <f>A16+1</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>21</v>
+        <v>57</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>22</v>
+        <v>8</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="F17" s="8">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <f>A17+1</f>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>33</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="E18" s="9"/>
       <c r="F18" s="8">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
-        <f>A18+1</f>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>35</v>
+        <v>8</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="F19" s="8">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
-        <f>A19+1</f>
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F20" s="8">
         <v>8</v>
@@ -1223,20 +1203,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
-        <f>A20+1</f>
-        <v>20</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>16</v>
+      <c r="D21" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="F21" s="8">
         <v>8</v>
@@ -1244,20 +1223,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
-        <f>A21+1</f>
-        <v>21</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F22" s="8">
         <v>13</v>
@@ -1265,121 +1243,119 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
-        <f>A22+1</f>
-        <v>22</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>29</v>
+        <v>4</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>31</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>47</v>
+        <v>7</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="F23" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
-        <f>A23+1</f>
-        <v>23</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>49</v>
+        <v>7</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="F24" s="8">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
-        <f>A24+1</f>
-        <v>24</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>16</v>
+      <c r="D25" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="F25" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
-        <f>A25+1</f>
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>63</v>
+        <v>7</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="F26" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
-        <f>A26+1</f>
+        <v>8</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="8"/>
+      <c r="F27" s="8">
+        <v>20</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
-        <f>A27+1</f>
-        <v>27</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>16</v>
+        <v>9</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="F28" s="8">
         <v>8</v>
@@ -1387,7 +1363,6 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
-        <f>A28+1</f>
         <v>28</v>
       </c>
       <c r="B29" s="7"/>
@@ -1397,29 +1372,46 @@
       <c r="F29" s="8"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="11">
-        <f>A29+1</f>
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="8"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="A31" s="11">
+        <v>30</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
   </sheetData>
   <sortState ref="A2:F31">
-    <sortCondition ref="D2:D31"/>
+    <sortCondition descending="1" ref="D2:D31"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D24 D30:D1048576">
+  <conditionalFormatting sqref="D1:D24 D31:D1048576">
     <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -1433,7 +1425,7 @@
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D29">
+  <conditionalFormatting sqref="D25:D30">
     <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -1462,7 +1454,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>"Sprint ready, Not sprint ready,Completed,In progress,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C33">
       <formula1>"High,Medium,Low,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Adding assignement to Sprint info
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -391,7 +391,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.14996795556505021"/>
@@ -791,7 +798,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:XFD28"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1412,42 +1419,47 @@
     <sortCondition descending="1" ref="D2:D31"/>
   </sortState>
   <conditionalFormatting sqref="D1:D24 D31:D1048576">
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:D30">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="BUG">
+      <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Sprint 8 creation and PB refinement
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -219,11 +219,11 @@
     <t>BUG: Clicking on a remove track does not stop playing file</t>
   </si>
   <si>
+    <t>Changing tone of the track inside track controls - referencing 24</t>
+  </si>
+  <si>
     <t>Removing track leaves loaded track playing, can not stop, and disable it 
-(referencing 9?)</t>
-  </si>
-  <si>
-    <t>Changing tone of the track inside track controls - referencing 24</t>
+(referencing ?)</t>
   </si>
 </sst>
 </file>
@@ -797,8 +797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,190 +954,188 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="F8" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
-        <v>26</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>64</v>
       </c>
       <c r="F9" s="8">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
-        <v>27</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="7" t="s">
-        <v>65</v>
+      <c r="E10" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="F10" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>18</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E11" s="9"/>
       <c r="F11" s="8">
-        <v>40</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>52</v>
       </c>
       <c r="F12" s="8">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F13" s="8">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="F14" s="8">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>58</v>
+        <v>28</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>50</v>
+        <v>17</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="F15" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>51</v>
+        <v>17</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="F16" s="8">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>29</v>
@@ -1145,29 +1143,31 @@
       <c r="D17" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="9"/>
+      <c r="E17" s="10" t="s">
+        <v>62</v>
+      </c>
       <c r="F17" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="8">
         <v>8</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="8">
-        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Edited PB and SI8
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\MasterAudioTechnologyFunctions\Documentation and designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djnenadovic\Desktop\MATF\MasterAudioTechnologyFunctions\Documentation and designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4452"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog user stories" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>Id</t>
   </si>
@@ -224,12 +224,21 @@
   <si>
     <t>Removing track leaves loaded track playing, can not stop, and disable it 
 (referencing ?)</t>
+  </si>
+  <si>
+    <t>All warning messages needs to be handled</t>
+  </si>
+  <si>
+    <t>Design buttons to follow new themes and styles</t>
+  </si>
+  <si>
+    <t>Create vector images all color combinations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -346,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -387,6 +396,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,24 +805,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="69" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="7" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -832,7 +842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>19</v>
       </c>
@@ -852,7 +862,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>20</v>
       </c>
@@ -872,7 +882,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>21</v>
       </c>
@@ -892,7 +902,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>22</v>
       </c>
@@ -912,7 +922,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>23</v>
       </c>
@@ -932,7 +942,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>24</v>
       </c>
@@ -952,7 +962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>26</v>
       </c>
@@ -972,7 +982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>27</v>
       </c>
@@ -992,7 +1002,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>12</v>
       </c>
@@ -1012,7 +1022,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>13</v>
       </c>
@@ -1030,7 +1040,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>14</v>
       </c>
@@ -1050,7 +1060,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>15</v>
       </c>
@@ -1070,7 +1080,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>16</v>
       </c>
@@ -1090,7 +1100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>17</v>
       </c>
@@ -1110,7 +1120,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>18</v>
       </c>
@@ -1130,212 +1140,212 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>25</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>62</v>
+        <v>28</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="F17" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
+        <v>29</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5">
+        <v>25</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
         <v>11</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>50</v>
-      </c>
-      <c r="F18" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>10</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>1</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>41</v>
       </c>
       <c r="F20" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>2</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="F21" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>3</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>31</v>
+        <v>1</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="F22" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="5">
+        <v>2</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>4</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="C23" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F23" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
+        <v>3</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="5">
         <v>4</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="B25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>6</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F25" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
-        <v>7</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>29</v>
+        <v>5</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="F26" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>30</v>
@@ -1344,18 +1354,18 @@
         <v>7</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F27" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>29</v>
@@ -1364,63 +1374,103 @@
         <v>7</v>
       </c>
       <c r="E28" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>8</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>9</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F30" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>28</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>29</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="11">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
         <v>30</v>
       </c>
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
+      <c r="B31"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="11">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F33">
-    <sortCondition descending="1" ref="D2:D33"/>
+  <sortState ref="A2:F34">
+    <sortCondition descending="1" ref="D2:D34"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D24 D31:D1048576">
+  <conditionalFormatting sqref="D1:D24 D33:D1048576">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -1434,7 +1484,7 @@
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D30">
+  <conditionalFormatting sqref="D25:D32">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -1468,7 +1518,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>"Sprint ready, Not sprint ready,Completed,In progress,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C33">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C35">
       <formula1>"High,Medium,Low,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added new story to sprint 8, updated PB
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -101,9 +101,6 @@
     <t>Implement final GUI design</t>
   </si>
   <si>
-    <t>For mp3, ogg, ac3, aiff, wma etc</t>
-  </si>
-  <si>
     <t>Custom, designed, implementation of GUI</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>BUG: Clicking on a remove track does not stop playing file</t>
   </si>
   <si>
-    <t>Changing tone of the track inside track controls - referencing 24</t>
-  </si>
-  <si>
     <t>Removing track leaves loaded track playing, can not stop, and disable it 
 (referencing ?)</t>
   </si>
@@ -233,6 +227,12 @@
   </si>
   <si>
     <t>Create vector images all color combinations</t>
+  </si>
+  <si>
+    <t>Changing tone of the track inside track controls - referencing 24 and 15</t>
+  </si>
+  <si>
+    <t>For mp3, ogg, ac3, aiff, wma etc (mimimum two of them)</t>
   </si>
 </sst>
 </file>
@@ -807,8 +807,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -839,7 +839,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -847,16 +847,16 @@
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="8">
         <v>8</v>
@@ -864,39 +864,39 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F3" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>40</v>
+      <c r="E4" s="9" t="s">
+        <v>46</v>
       </c>
       <c r="F4" s="8">
         <v>13</v>
@@ -904,10 +904,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>29</v>
@@ -916,7 +916,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F5" s="8">
         <v>13</v>
@@ -924,177 +924,177 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>23</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="9" t="s">
-        <v>49</v>
+      <c r="E6" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="F6" s="8">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>24</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="7" t="s">
-        <v>54</v>
+      <c r="E7" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="F7" s="8">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>26</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>65</v>
+      <c r="E8" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="F8" s="8">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>27</v>
-      </c>
-      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>64</v>
+      <c r="E9" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="F9" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>56</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>51</v>
-      </c>
+      <c r="E10" s="9"/>
       <c r="F10" s="8">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="F11" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>52</v>
+        <v>17</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F12" s="8">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F13" s="8">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="F14" s="8">
         <v>20</v>
@@ -1102,82 +1102,82 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F15" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>18</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F16" s="8">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>28</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>66</v>
+        <v>29</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>65</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="F17" s="8">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
+        <v>20</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>17</v>
+      <c r="D18" s="9" t="s">
+        <v>8</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>68</v>
       </c>
       <c r="F18" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1185,16 +1185,16 @@
         <v>25</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F19" s="8">
         <v>5</v>
@@ -1205,16 +1205,16 @@
         <v>11</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F20" s="8">
         <v>8</v>
@@ -1225,16 +1225,16 @@
         <v>10</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F21" s="8">
         <v>3</v>
@@ -1248,13 +1248,13 @@
         <v>12</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F22" s="8">
         <v>8</v>
@@ -1268,7 +1268,7 @@
         <v>13</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>7</v>
@@ -1288,7 +1288,7 @@
         <v>5</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>7</v>
@@ -1308,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="C25" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>7</v>
@@ -1328,7 +1328,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>7</v>
@@ -1348,7 +1348,7 @@
         <v>19</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>7</v>
@@ -1365,16 +1365,16 @@
         <v>7</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F28" s="8">
         <v>5</v>
@@ -1388,13 +1388,13 @@
         <v>24</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F29" s="8">
         <v>20</v>
@@ -1405,16 +1405,16 @@
         <v>9</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F30" s="8">
         <v>8</v>
@@ -1467,8 +1467,8 @@
       <c r="F35" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F34">
-    <sortCondition descending="1" ref="D2:D34"/>
+  <sortState ref="A2:F35">
+    <sortCondition descending="1" ref="D2:D35"/>
   </sortState>
   <conditionalFormatting sqref="D1:D24 D33:D1048576">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">

</xml_diff>

<commit_message>
Edited Sprint8. Edited PB.
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -232,7 +232,7 @@
     <t>Changing tone of the track inside track controls - referencing 24 and 15</t>
   </si>
   <si>
-    <t>For mp3, ogg, ac3, aiff, wma etc (mimimum two of them)</t>
+    <t>For mp3, ogg, ac3, aiff, wma etc (mimimum mp3)</t>
   </si>
 </sst>
 </file>
@@ -808,17 +808,17 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="69" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
@@ -942,7 +942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>26</v>
       </c>
@@ -962,7 +962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>27</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>29</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>20</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>25</v>
       </c>
@@ -1200,7 +1200,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Created new sprint and added changes to PB
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -808,7 +808,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -984,137 +984,137 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>50</v>
-      </c>
+      <c r="E9" s="9"/>
       <c r="F9" s="8">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="9"/>
+        <v>17</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="F10" s="8">
-        <v>8</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>51</v>
+        <v>17</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="F11" s="8">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="F12" s="8">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F13" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
+        <v>28</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="F14" s="8">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="F15" s="8">
         <v>13</v>
@@ -1122,19 +1122,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>28</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>37</v>
+        <v>12</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="F16" s="8">
         <v>5</v>
@@ -1142,22 +1142,22 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>66</v>
+      <c r="D17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="F17" s="8">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,7 +1191,7 @@
         <v>28</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>61</v>
@@ -1467,8 +1467,8 @@
       <c r="F35" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F35">
-    <sortCondition descending="1" ref="D2:D35"/>
+  <sortState ref="A2:F33">
+    <sortCondition descending="1" ref="D2:D33"/>
   </sortState>
   <conditionalFormatting sqref="D1:D24 D33:D1048576">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">

</xml_diff>

<commit_message>
Edited Sprint info files and PB
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="71">
   <si>
     <t>Id</t>
   </si>
@@ -233,6 +233,12 @@
   </si>
   <si>
     <t>For mp3, ogg, ac3, aiff, wma etc (mimimum mp3)</t>
+  </si>
+  <si>
+    <t>Add support for custom sound file formats</t>
+  </si>
+  <si>
+    <t>Implement support for other audio file formats</t>
   </si>
 </sst>
 </file>
@@ -805,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -844,19 +850,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>19</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="F2" s="8">
         <v>8</v>
@@ -864,50 +870,48 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="E3" s="9"/>
       <c r="F3" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>22</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>46</v>
+      <c r="E4" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="F4" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>29</v>
@@ -915,8 +919,8 @@
       <c r="D5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>48</v>
+      <c r="E5" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="F5" s="8">
         <v>13</v>
@@ -924,70 +928,70 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>24</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>53</v>
+      <c r="E6" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="F6" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>26</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>63</v>
+      <c r="E7" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="F7" s="8">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>27</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>67</v>
+      <c r="E8" s="10" t="s">
+        <v>63</v>
       </c>
       <c r="F8" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>28</v>
@@ -995,29 +999,31 @@
       <c r="D9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9"/>
+      <c r="E9" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="F9" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>17</v>
+      <c r="D10" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
       <c r="F10" s="8">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1042,30 +1048,30 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
+        <v>29</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="F12" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>29</v>
@@ -1074,78 +1080,78 @@
         <v>17</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" s="8">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>28</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="9" t="s">
         <v>17</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F14" s="8">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
+        <v>28</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="F15" s="8">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>50</v>
+        <v>17</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="F16" s="8">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>30</v>
@@ -1154,127 +1160,127 @@
         <v>8</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F17" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="7" t="s">
-        <v>68</v>
+      <c r="E18" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="F18" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>61</v>
+      <c r="E19" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="F19" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>11</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>49</v>
+      <c r="E20" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="F20" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>10</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="F21" s="8">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="F22" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
-        <v>2</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
       <c r="F23" s="8">
         <v>8</v>
@@ -1282,39 +1288,39 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
-        <v>3</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>10</v>
+      <c r="E24" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="F24" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
-        <v>4</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F25" s="8">
         <v>8</v>
@@ -1322,30 +1328,30 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
-        <v>5</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F26" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>29</v>
@@ -1354,18 +1360,18 @@
         <v>7</v>
       </c>
       <c r="E27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="8">
         <v>20</v>
-      </c>
-      <c r="F27" s="8">
-        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>28</v>
@@ -1373,8 +1379,8 @@
       <c r="D28" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>43</v>
+      <c r="E28" s="10" t="s">
+        <v>61</v>
       </c>
       <c r="F28" s="8">
         <v>5</v>
@@ -1382,30 +1388,30 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="8">
         <v>8</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="8">
-        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>28</v>
@@ -1414,21 +1420,31 @@
         <v>7</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="F30" s="8">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>30</v>
-      </c>
-      <c r="B31"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="8"/>
+        <v>9</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="8">
+        <v>8</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
@@ -1441,22 +1457,24 @@
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="11">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="13"/>
+      <c r="B33"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
+      <c r="A34" s="11">
+        <v>33</v>
+      </c>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7"/>
@@ -1466,11 +1484,20 @@
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
     </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:F33">
-    <sortCondition descending="1" ref="D2:D33"/>
+  <sortState ref="A2:F36">
+    <sortCondition descending="1" ref="D2:D36"/>
+    <sortCondition ref="C2:C36" customList="High,Medium,Low"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D24 D33:D1048576">
+  <conditionalFormatting sqref="D1:D24 D34:D1048576">
     <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -1484,7 +1511,7 @@
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D32">
+  <conditionalFormatting sqref="D25:D33">
     <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
@@ -1518,7 +1545,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>"Sprint ready, Not sprint ready,Completed,In progress,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C35">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C36">
       <formula1>"High,Medium,Low,"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added one user story to sprint, edited PB and Sprint info 9
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -822,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -859,39 +859,39 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>72</v>
+        <v>17</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="F2" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
-        <v>27</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>53</v>
+        <v>29</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="F3" s="8">
         <v>8</v>
@@ -899,39 +899,39 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
-        <v>19</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>16</v>
+      <c r="D4" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="F4" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F5" s="8">
         <v>13</v>
@@ -939,159 +939,159 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
-        <v>23</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>47</v>
+      <c r="D6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="F6" s="8">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
-        <v>24</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>17</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="F7" s="8">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>62</v>
+      <c r="E8" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="F8" s="8">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>22</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>45</v>
+      <c r="E9" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="F9" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>30</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>29</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="F10" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
+        <v>21</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>17</v>
-      </c>
       <c r="E11" s="7" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="F11" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
+        <v>23</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>71</v>
+      <c r="D12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="F12" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>17</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>17</v>
+      <c r="D13" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="F13" s="8">
         <v>20</v>
@@ -1099,19 +1099,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>33</v>
+        <v>16</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="F14" s="8">
         <v>13</v>
@@ -1119,50 +1119,50 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
+        <v>30</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>17</v>
+      <c r="D15" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F15" s="8">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="F16" s="8">
-        <v>40</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>30</v>
@@ -1171,27 +1171,27 @@
         <v>8</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F17" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>50</v>
+      <c r="E18" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="F18" s="8">
         <v>3</v>
@@ -1199,130 +1199,130 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>3</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>48</v>
       </c>
       <c r="F19" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F20" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>5</v>
-      </c>
-      <c r="B21" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="B21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F21" s="8">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>10</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F22" s="8">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
-        <v>2</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="F23" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
-        <v>6</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F24" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>29</v>
@@ -1331,30 +1331,30 @@
         <v>7</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F25" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>56</v>
+        <v>24</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>48</v>
+        <v>7</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F26" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1505,7 +1505,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:F36">
-    <sortCondition descending="1" ref="D2:D36"/>
+    <sortCondition descending="1" ref="D2:D36" customList="Completed,Outdated,In progress,Sprint ready,Not sprint ready"/>
     <sortCondition ref="C2:C36" customList="High,Medium,Low"/>
     <sortCondition ref="A2:A36"/>
   </sortState>

</xml_diff>

<commit_message>
Edited PB, added progress chart
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4452"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4452" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog user stories" sheetId="1" r:id="rId1"/>
+    <sheet name="Progress chart" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="79">
   <si>
     <t>Id</t>
   </si>
@@ -248,13 +249,29 @@
   </si>
   <si>
     <t>Outdated</t>
+  </si>
+  <si>
+    <t>Implement timescale for timeline</t>
+  </si>
+  <si>
+    <t>Timescale should simplify editing timeline, and enable user to put 
+wav file to specific place</t>
+  </si>
+  <si>
+    <t>Complete effort</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>To do</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +280,33 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,8 +319,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -366,11 +423,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -412,11 +502,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -504,6 +616,13 @@
         <color theme="7" tint="-0.24994659260841701"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -521,6 +640,936 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="sr-Latn-RS"/>
+              <a:t>Progress chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent2">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="95000"/>
+                      <a:alpha val="54000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Progress chart'!$B$1:$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Done</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>To do</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Progress chart'!$B$2:$C$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>210</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="1"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="257">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>388620</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -820,10 +1869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,7 +1883,11 @@
     <col min="4" max="4" width="14.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="67.44140625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="4"/>
+    <col min="7" max="7" width="9.109375" style="4"/>
+    <col min="8" max="8" width="14.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -957,61 +2010,61 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
+        <v>31</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>15</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F8" s="8">
         <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>13</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="8">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>27</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>64</v>
+      <c r="E9" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="F9" s="8">
         <v>8</v>
@@ -1019,19 +2072,19 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>19</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>30</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="F10" s="8">
         <v>8</v>
@@ -1039,30 +2092,30 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>21</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F11" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>29</v>
@@ -1070,8 +2123,8 @@
       <c r="D12" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>47</v>
+      <c r="E12" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="F12" s="8">
         <v>13</v>
@@ -1079,59 +2132,59 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>24</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="7" t="s">
-        <v>52</v>
+      <c r="E13" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="F13" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>22</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>45</v>
+      <c r="E14" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="F14" s="8">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>69</v>
+      <c r="E15" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="F15" s="8">
         <v>13</v>
@@ -1139,30 +2192,30 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>49</v>
+        <v>66</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="F16" s="8">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>30</v>
@@ -1171,178 +2224,178 @@
         <v>8</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F17" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>62</v>
+      <c r="E18" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="F18" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>11</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E20" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F20" s="8">
         <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>3</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="8">
-        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F21" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>5</v>
-      </c>
-      <c r="B22" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="B22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F22" s="8">
-        <v>20</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
-        <v>10</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C23" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="F23" s="8">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
-        <v>2</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="F24" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
+        <v>2</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
         <v>6</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B26" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>8</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>24</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>29</v>
@@ -1351,18 +2404,18 @@
         <v>7</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F26" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>29</v>
@@ -1371,27 +2424,27 @@
         <v>7</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F27" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
-        <v>1</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="F28" s="8">
         <v>8</v>
@@ -1399,30 +2452,30 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
+        <v>1</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>7</v>
-      </c>
       <c r="E29" s="7" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F29" s="8">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>28</v>
@@ -1431,18 +2484,18 @@
         <v>7</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="F30" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>28</v>
@@ -1450,22 +2503,32 @@
       <c r="D31" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="10" t="s">
+      <c r="E31" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>25</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="8">
+      <c r="F32" s="8">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
-        <v>31</v>
-      </c>
-      <c r="B32"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
@@ -1478,22 +2541,24 @@
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="11">
+      <c r="A34" s="5">
         <v>33</v>
       </c>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
+      <c r="B34"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="A35" s="11">
+        <v>34</v>
+      </c>
+      <c r="B35" s="12"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="13"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="7"/>
@@ -1503,53 +2568,61 @@
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
   </sheetData>
-  <sortState ref="A2:F36">
-    <sortCondition descending="1" ref="D2:D36" customList="Completed,Outdated,In progress,Sprint ready,Not sprint ready"/>
-    <sortCondition ref="C2:C36" customList="High,Medium,Low"/>
-    <sortCondition ref="A2:A36"/>
+  <sortState ref="A2:F37">
+    <sortCondition descending="1" ref="D2:D37" customList="Completed,Outdated,In progress,Sprint ready,Not sprint ready"/>
+    <sortCondition ref="C2:C37" customList="High,Medium,Low"/>
+    <sortCondition ref="A2:A37"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D24 D34:D1048576">
-    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
+  <conditionalFormatting sqref="D1:D24 D35:D1048576">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D33">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+  <conditionalFormatting sqref="D25:D34">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="BUG">
+  <conditionalFormatting sqref="A1:XFD2 A5:XFD1048576 A3:G4 K3:XFD4">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1557,11 +2630,62 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>"Sprint ready, Not sprint ready,Completed,In progress,Outdated,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C36">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C37">
       <formula1>"High,Medium,Low,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18">
+        <f>SUM('Backlog user stories'!F:F)</f>
+        <v>348</v>
+      </c>
+      <c r="B2" s="18">
+        <f>SUMIF('Backlog user stories'!D:D,"Completed",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Outdated",'Backlog user stories'!F:F)</f>
+        <v>127</v>
+      </c>
+      <c r="C2" s="18">
+        <f>SUMIF('Backlog user stories'!D:D,"Not sprint ready",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Sprint ready",'Backlog user stories'!F:F)</f>
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:C2">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="BUG">
+      <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed small grammar errors in document
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -270,7 +270,7 @@
     <t>BUG: Time progress label is starting even if no tracks is loaded</t>
   </si>
   <si>
-    <t>It stars on pressing burron play</t>
+    <t>It starts on pressing button play</t>
   </si>
 </sst>
 </file>
@@ -513,14 +513,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -1863,8 +1856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2595,46 +2588,46 @@
     <sortCondition ref="A2:A38"/>
   </sortState>
   <conditionalFormatting sqref="D1:D24 D36:D1048576">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:D35">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD2 A3:G4 K3:XFD4 A5:XFD1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2693,7 +2686,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C2">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Created sprint10 and edited PB
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="85">
   <si>
     <t>Id</t>
   </si>
@@ -271,6 +271,18 @@
   </si>
   <si>
     <t>It starts on pressing button play</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Move edit buttons from Track to Timeline</t>
+  </si>
+  <si>
+    <t>Refactor select to edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BUG: Sound doesn't play when it not visible inside window </t>
   </si>
 </sst>
 </file>
@@ -513,7 +525,14 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -608,6 +627,45 @@
         <color theme="7" tint="-0.24994659260841701"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="8" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -673,6 +731,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -851,7 +910,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -875,10 +936,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>128</c:v>
+                  <c:v>139</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>210</c:v>
+                  <c:v>194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -906,6 +967,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1850,10 +1912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2033,19 +2095,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
-        <v>13</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>72</v>
+      <c r="E9" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="F9" s="8">
         <v>8</v>
@@ -2053,79 +2115,79 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
-        <v>27</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="F10" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
-        <v>19</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>41</v>
+      <c r="E11" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="F11" s="8">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
-        <v>21</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F12" s="8">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="8">
         <v>13</v>
@@ -2133,230 +2195,230 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
-        <v>24</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>51</v>
+        <v>30</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="F14" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="F15" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
+        <v>27</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>28</v>
-      </c>
       <c r="D16" s="7" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="F16" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E17" s="9" t="s">
-        <v>49</v>
+      <c r="E17" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="F17" s="8">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>50</v>
+      <c r="E18" s="7" t="s">
+        <v>83</v>
       </c>
       <c r="F18" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="8">
         <v>8</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="5">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>48</v>
+      <c r="E20" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="F20" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
-        <v>32</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>79</v>
+        <v>3</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="F21" s="8">
-        <v>1</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F22" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
+        <v>5</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="F23" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
-        <v>5</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F24" s="8">
-        <v>20</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>30</v>
@@ -2364,59 +2426,59 @@
       <c r="D25" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>36</v>
+      <c r="E25" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="F25" s="8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
-        <v>2</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>9</v>
+      <c r="E26" s="9" t="s">
+        <v>50</v>
       </c>
       <c r="F26" s="8">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
-        <v>6</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F27" s="8">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>29</v>
@@ -2425,18 +2487,18 @@
         <v>7</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="F28" s="8">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>29</v>
@@ -2445,78 +2507,78 @@
         <v>7</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F29" s="8">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
-        <v>1</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D30" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="F30" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>42</v>
+      <c r="E31" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="F31" s="8">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
-        <v>9</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="9" t="s">
+      <c r="D32" s="7" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="F32" s="8">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>28</v>
@@ -2524,8 +2586,8 @@
       <c r="D33" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="10" t="s">
-        <v>60</v>
+      <c r="E33" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="F33" s="8">
         <v>5</v>
@@ -2533,97 +2595,137 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
-        <v>33</v>
-      </c>
-      <c r="B34"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
-        <v>34</v>
-      </c>
-      <c r="B35"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="12"/>
+      <c r="B36"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="12"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F38">
-    <sortCondition descending="1" ref="D2:D38" customList="Completed,Outdated,In progress,Sprint ready,Not sprint ready"/>
-    <sortCondition ref="C2:C38" customList="High,Medium,Low"/>
-    <sortCondition ref="A2:A38"/>
+  <sortState ref="A2:F40">
+    <sortCondition descending="1" ref="D2:D40" customList="Completed,Outdated,In progress,Sprint ready,Not sprint ready"/>
+    <sortCondition ref="C2:C40" customList="High,Medium,Low"/>
+    <sortCondition ref="A2:A40"/>
   </sortState>
-  <conditionalFormatting sqref="D1:D24 D36:D1048576">
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+  <conditionalFormatting sqref="D38:D1048576 D1:D24">
+    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25:D35">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
+  <conditionalFormatting sqref="D25:D37">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD2 A3:G4 K3:XFD4 A5:XFD1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2631,7 +2733,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576">
       <formula1>"Sprint ready, Not sprint ready,Completed,In progress,Outdated,"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C40">
       <formula1>"High,Medium,Low,"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2669,20 +2771,20 @@
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <f>SUM('Backlog user stories'!F:F)</f>
-        <v>349</v>
+        <v>359</v>
       </c>
       <c r="B2" s="17">
         <f>SUMIF('Backlog user stories'!D:D,"Completed",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Outdated",'Backlog user stories'!F:F)</f>
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C2" s="17">
         <f>SUMIF('Backlog user stories'!D:D,"Not sprint ready",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Sprint ready",'Backlog user stories'!F:F)</f>
-        <v>210</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C2">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Edited Sprint10 info and PB, cosmetic changes
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -282,7 +282,7 @@
     <t>Refactor select to edit</t>
   </si>
   <si>
-    <t xml:space="preserve">BUG: Sound doesn't play when it not visible inside window </t>
+    <t xml:space="preserve">BUG: Sound doesn't play when it's not visible inside window </t>
   </si>
 </sst>
 </file>
@@ -525,14 +525,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="13">
     <dxf>
       <fill>
         <patternFill>
@@ -601,45 +594,6 @@
       <font>
         <color theme="7" tint="-0.24994659260841701"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="8" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1915,7 +1869,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2686,46 +2640,46 @@
     <sortCondition ref="A2:A40"/>
   </sortState>
   <conditionalFormatting sqref="D38:D1048576 D1:D24">
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:D37">
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Not sprint ready"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"Sprint ready"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Low">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Low">
       <formula>NOT(ISERROR(SEARCH("Low",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD2 A3:G4 K3:XFD4 A5:XFD1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2784,7 +2738,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:C2">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="BUG">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="BUG">
       <formula>NOT(ISERROR(SEARCH("BUG",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Sprint 10 and PB update
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -183,9 +183,6 @@
     <t>Implement various sound effects</t>
   </si>
   <si>
-    <t>Changing of frequency, etc...</t>
-  </si>
-  <si>
     <t xml:space="preserve">Implement frequention changing per track </t>
   </si>
   <si>
@@ -283,6 +280,9 @@
   </si>
   <si>
     <t xml:space="preserve">BUG: Sound doesn't play when it's not visible inside window </t>
+  </si>
+  <si>
+    <t>Changing of frequency, echo, fade in, fade out, etc...</t>
   </si>
 </sst>
 </file>
@@ -353,80 +353,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -460,28 +391,96 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -490,33 +489,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -685,7 +706,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -864,9 +884,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -921,7 +939,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="l"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1869,769 +1886,769 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="4"/>
-    <col min="8" max="8" width="14.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.109375" style="1"/>
+    <col min="8" max="8" width="14.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5">
+      <c r="A2" s="16">
         <v>16</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="15">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="A3" s="16">
         <v>29</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="F3" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="16">
+        <v>17</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="16">
+        <v>18</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="16">
+        <v>28</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="16">
+        <v>31</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="16">
+        <v>15</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="16">
+        <v>21</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="7" t="s">
+      <c r="D9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="16">
+        <v>19</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="16">
+        <v>23</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="16">
+        <v>24</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="16">
+        <v>22</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F13" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="16">
+        <v>30</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
+        <v>13</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F15" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>17</v>
-      </c>
-      <c r="B4" s="10" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="16">
         <v>27</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="B16" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="16">
+        <v>33</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F17" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="16">
+        <v>34</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="D18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="F18" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="16">
+        <v>11</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="16">
+        <v>32</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="16">
+        <v>3</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="16">
+        <v>4</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
+        <v>5</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="15">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
-        <v>18</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="10" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="16">
+        <v>10</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
+        <v>12</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="16">
+        <v>14</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="16">
+        <v>2</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="8">
+      <c r="D27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="16">
+        <v>6</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="15">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="16">
+        <v>8</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="16">
+        <v>20</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F30" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="16">
+        <v>26</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="F31" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="16">
+        <v>1</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="D32" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F32" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="16">
+        <v>7</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>31</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F7" s="8">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
+        <v>9</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34" s="15">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>15</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="10" t="s">
+    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
+        <v>25</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
-        <v>19</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5">
-        <v>21</v>
-      </c>
-      <c r="B10" s="10" t="s">
+      <c r="D35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F35" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="16">
+        <v>35</v>
+      </c>
+      <c r="B36" s="18"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="15"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="16">
+        <v>36</v>
+      </c>
+      <c r="B37" s="18"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="15"/>
+    </row>
+    <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="19">
         <v>37</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>23</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>24</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5">
-        <v>22</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="5">
-        <v>30</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
-        <v>13</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
-        <v>27</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
-        <v>33</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5">
-        <v>34</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>11</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F19" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
-        <v>32</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="F20" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
-        <v>3</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="5">
-        <v>4</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F22" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="5">
-        <v>5</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5">
-        <v>10</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F24" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="5">
-        <v>12</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="5">
-        <v>14</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F26" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5">
-        <v>2</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="5">
-        <v>6</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="8">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="5">
-        <v>8</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="8">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="5">
-        <v>20</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F30" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A31" s="5">
-        <v>26</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" s="8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="5">
-        <v>1</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="5">
-        <v>7</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="F33" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
-        <v>9</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F34" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
-        <v>25</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="F35" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="5">
-        <v>35</v>
-      </c>
-      <c r="B36"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="5">
-        <v>36</v>
-      </c>
-      <c r="B37"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="5">
-        <v>37</v>
-      </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="12"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="21"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:F40">
@@ -2712,26 +2729,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>78</v>
-      </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17">
+      <c r="A2" s="10">
         <f>SUM('Backlog user stories'!F:F)</f>
         <v>359</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="10">
         <f>SUMIF('Backlog user stories'!D:D,"Completed",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Outdated",'Backlog user stories'!F:F)</f>
         <v>139</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="10">
         <f>SUMIF('Backlog user stories'!D:D,"Not sprint ready",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Sprint ready",'Backlog user stories'!F:F)</f>
         <v>194</v>
       </c>

</xml_diff>

<commit_message>
Sprint11 creation and PB refining
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -913,10 +913,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>139</c:v>
+                  <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>197</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1890,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2071,10 +2071,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>30</v>
@@ -2082,68 +2082,68 @@
       <c r="D9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>38</v>
+      <c r="E9" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="F9" s="14">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
-        <v>35</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
+        <v>19</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>86</v>
+      <c r="E10" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F10" s="14">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
-        <v>19</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="F11" s="14">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>47</v>
+      <c r="E12" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F12" s="14">
         <v>13</v>
@@ -2151,59 +2151,59 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
-        <v>24</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="F13" s="14">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
-        <v>22</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="F14" s="14">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>68</v>
+        <v>44</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F15" s="14">
         <v>13</v>
@@ -2211,59 +2211,59 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="4" t="s">
-        <v>71</v>
+      <c r="E16" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="F16" s="14">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>63</v>
+        <v>72</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="F17" s="14">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>80</v>
+        <v>55</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F18" s="14">
         <v>8</v>
@@ -2271,130 +2271,130 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>8</v>
+        <v>72</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F19" s="14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
-        <v>11</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>48</v>
+        <v>3</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F20" s="14">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
-        <v>32</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>78</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>72</v>
+        <v>30</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="F21" s="14">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
-        <v>3</v>
-      </c>
-      <c r="B22" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="B22" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F22" s="14">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
-        <v>4</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F23" s="14">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
-        <v>5</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>14</v>
+      <c r="E24" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="F24" s="14">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>30</v>
@@ -2402,19 +2402,19 @@
       <c r="D25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>36</v>
+      <c r="E25" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="F25" s="14">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>30</v>
@@ -2423,30 +2423,30 @@
         <v>7</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F26" s="14">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>50</v>
+      <c r="E27" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="F27" s="14">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2771,11 +2771,11 @@
       </c>
       <c r="B2" s="9">
         <f>SUMIF('Backlog user stories'!D:D,"Completed",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Outdated",'Backlog user stories'!F:F)</f>
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="C2" s="9">
         <f>SUMIF('Backlog user stories'!D:D,"Not sprint ready",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Sprint ready",'Backlog user stories'!F:F)</f>
-        <v>197</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Sprint12 and PB edited
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -916,7 +916,7 @@
                   <c:v>158</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>168</c:v>
+                  <c:v>132</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1890,8 +1890,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1931,19 +1931,19 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="F2" s="14">
         <v>20</v>
@@ -1951,99 +1951,99 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
+        <v>18</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="F3" s="14">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
+        <v>28</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F4" s="14">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F5" s="14">
-        <v>13</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
-        <v>28</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>66</v>
+        <v>23</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="F6" s="14">
-        <v>5</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
-        <v>31</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>74</v>
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="F7" s="14">
         <v>8</v>
@@ -2051,39 +2051,39 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
-        <v>15</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="F8" s="14">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>47</v>
+      <c r="E9" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F9" s="14">
         <v>13</v>
@@ -2091,122 +2091,122 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
-        <v>19</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="B10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="E10" s="3" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="F10" s="14">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
-        <v>24</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>84</v>
+        <v>38</v>
       </c>
       <c r="F11" s="14">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
+        <v>27</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F12" s="14">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="F13" s="14">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
-        <v>27</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>63</v>
+      <c r="E14" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F14" s="14">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>45</v>
+      <c r="E15" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="F15" s="14">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2676,7 +2676,7 @@
       <c r="F41" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F41">
+  <sortState ref="A2:J41">
     <sortCondition descending="1" ref="D2:D41" customList="Completed,Outdated,In progress,Sprint ready,Not sprint ready"/>
     <sortCondition ref="C2:C41" customList="High,Medium,Low"/>
     <sortCondition ref="A2:A41"/>
@@ -2775,7 +2775,7 @@
       </c>
       <c r="C2" s="9">
         <f>SUMIF('Backlog user stories'!D:D,"Not sprint ready",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Sprint ready",'Backlog user stories'!F:F)</f>
-        <v>168</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added last sprint infos
</commit_message>
<xml_diff>
--- a/Documentation and designs/Product Backlog.xlsx
+++ b/Documentation and designs/Product Backlog.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djnenadovic\Desktop\MATF\MasterAudioTechnologyFunctions\Documentation and designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\GIT\MasterAudioTechnologyFunctions\Documentation and designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4452"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog user stories" sheetId="1" r:id="rId1"/>
     <sheet name="Progress chart" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -295,7 +295,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -666,7 +666,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -742,7 +742,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sr-Latn-RS"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -795,6 +795,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3238-4FAA-97BB-4B55D9970180}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -837,6 +842,11 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3238-4FAA-97BB-4B55D9970180}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:spPr>
@@ -864,7 +874,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="sr-Latn-RS"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -913,7 +923,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>158</c:v>
+                  <c:v>222</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>132</c:v>
@@ -921,6 +931,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3238-4FAA-97BB-4B55D9970180}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="outEnd"/>
@@ -968,7 +983,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="sr-Latn-RS"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1009,7 +1024,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="sr-Latn-RS"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1891,25 +1906,25 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="67.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
-    <col min="8" max="8" width="14.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="56.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="67.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.125" style="1"/>
+    <col min="8" max="8" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1929,7 +1944,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>17</v>
       </c>
@@ -1949,7 +1964,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
         <v>18</v>
       </c>
@@ -1969,7 +1984,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>28</v>
       </c>
@@ -1989,7 +2004,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>15</v>
       </c>
@@ -2009,7 +2024,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>23</v>
       </c>
@@ -2029,7 +2044,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>19</v>
       </c>
@@ -2049,7 +2064,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>24</v>
       </c>
@@ -2069,7 +2084,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
         <v>30</v>
       </c>
@@ -2089,392 +2104,392 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
-        <v>16</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>22</v>
+        <v>63</v>
       </c>
       <c r="F10" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
-        <v>21</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>38</v>
+      <c r="D11" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="F11" s="14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
-        <v>27</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>63</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="F12" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
+        <v>32</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <v>3</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="15">
-        <v>22</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>45</v>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="F14" s="14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
-        <v>31</v>
-      </c>
-      <c r="B15" s="13" t="s">
-        <v>73</v>
+        <v>4</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>6</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>74</v>
+        <v>30</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="F15" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
-        <v>34</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>82</v>
+        <v>14</v>
       </c>
       <c r="F16" s="14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
-        <v>35</v>
-      </c>
-      <c r="B17" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>86</v>
+      <c r="D17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="F17" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F18" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>13</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F19" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="15">
-        <v>32</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F19" s="14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
+        <v>14</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F20" s="14">
         <v>3</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
-        <v>4</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F21" s="14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
-        <v>5</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
       <c r="F22" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C23" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="F23" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="C24" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>49</v>
+      <c r="E24" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="F24" s="14">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
+        <v>2</v>
+      </c>
+      <c r="B25" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="4" t="s">
+      <c r="C25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>71</v>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="F25" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>50</v>
+      <c r="E26" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="F26" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="F27" s="14">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
-        <v>2</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="F28" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>29</v>
@@ -2482,19 +2497,19 @@
       <c r="D29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>20</v>
+      <c r="E29" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="F29" s="14">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>29</v>
@@ -2502,54 +2517,54 @@
       <c r="D30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>25</v>
+      <c r="E30" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="F30" s="14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>64</v>
+      <c r="E31" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="F31" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>61</v>
+      <c r="E32" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="F32" s="14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>1</v>
       </c>
@@ -2569,7 +2584,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="15">
         <v>7</v>
       </c>
@@ -2589,7 +2604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15">
         <v>9</v>
       </c>
@@ -2609,7 +2624,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>25</v>
       </c>
@@ -2629,7 +2644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <v>36</v>
       </c>
@@ -2639,7 +2654,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="14"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <v>37</v>
       </c>
@@ -2649,7 +2664,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="14"/>
     </row>
-    <row r="39" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="15">
         <v>38</v>
       </c>
@@ -2659,7 +2674,7 @@
       <c r="E39" s="18"/>
       <c r="F39" s="19"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -2667,7 +2682,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2676,7 +2691,7 @@
       <c r="F41" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:J41">
+  <sortState ref="A2:F41">
     <sortCondition descending="1" ref="D2:D41" customList="Completed,Outdated,In progress,Sprint ready,Not sprint ready"/>
     <sortCondition ref="C2:C41" customList="High,Medium,Low"/>
     <sortCondition ref="A2:A41"/>
@@ -2746,14 +2761,14 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>75</v>
       </c>
@@ -2764,14 +2779,14 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <f>SUM('Backlog user stories'!F:F)</f>
         <v>362</v>
       </c>
       <c r="B2" s="9">
         <f>SUMIF('Backlog user stories'!D:D,"Completed",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Outdated",'Backlog user stories'!F:F)</f>
-        <v>158</v>
+        <v>222</v>
       </c>
       <c r="C2" s="9">
         <f>SUMIF('Backlog user stories'!D:D,"Not sprint ready",'Backlog user stories'!F:F)+SUMIF('Backlog user stories'!D:D,"Sprint ready",'Backlog user stories'!F:F)</f>

</xml_diff>